<commit_message>
Multistate oscillator fully translated into objected oriented framework.
</commit_message>
<xml_diff>
--- a/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Multistate_CPG_Phase_Alignment/Robot_Data/Neuron_Data.xlsx
+++ b/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Multistate_CPG_Phase_Alignment/Robot_Data/Neuron_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody Scharzenberger\Documents\GitHub\Quadruped_Robot\Code\Matlab\Quadruped_Simulation\Quadruped_Simulation_Framework\Main\Simulation\Software\Multistate_CPG_Phase_Alignment\Robot_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2032CF65-8967-4B07-82B6-CD92579E1A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132BF028-2304-4001-9E71-1C6214B39446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB897387-95F6-4630-A620-05952313E6EB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>CPG 4</t>
+  </si>
+  <si>
+    <t>Initial Voltage</t>
+  </si>
+  <si>
+    <t>U0</t>
   </si>
 </sst>
 </file>
@@ -290,9 +296,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1"/>
@@ -303,6 +306,9 @@
     <xf numFmtId="11" fontId="1" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="8" borderId="1" xfId="7" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="10" borderId="1" xfId="9" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -627,360 +633,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6662B30-3957-4791-B63A-8C16E3B479F3}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="P2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
         <v>5.0000000000000001E-9</v>
       </c>
-      <c r="D4" s="13">
+      <c r="E4" s="12">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E4" s="13">
+      <c r="F4" s="12">
         <v>-0.06</v>
       </c>
-      <c r="F4" s="13">
+      <c r="G4" s="12">
         <v>0.02</v>
       </c>
-      <c r="G4" s="14">
+      <c r="H4" s="13">
         <v>1</v>
       </c>
-      <c r="H4" s="14">
+      <c r="I4" s="13">
         <v>-50</v>
       </c>
-      <c r="I4" s="14">
-        <f>2*F4</f>
+      <c r="J4" s="13">
+        <f>2*G4</f>
         <v>0.04</v>
       </c>
-      <c r="J4" s="15">
+      <c r="K4" s="14">
         <v>0.5</v>
       </c>
-      <c r="K4" s="15">
+      <c r="L4" s="14">
         <v>50</v>
       </c>
-      <c r="L4" s="15">
-        <v>0</v>
-      </c>
-      <c r="M4" s="16">
+      <c r="M4" s="14">
+        <v>0</v>
+      </c>
+      <c r="N4" s="15">
         <v>0.11</v>
       </c>
-      <c r="N4" s="16">
+      <c r="O4" s="15">
         <v>0.25</v>
       </c>
-      <c r="O4" s="16">
+      <c r="P4" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
         <v>5.0000000000000001E-9</v>
       </c>
-      <c r="D5" s="13">
+      <c r="E5" s="12">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E5" s="13">
+      <c r="F5" s="12">
         <v>-0.06</v>
       </c>
-      <c r="F5" s="13">
+      <c r="G5" s="12">
         <v>0.02</v>
       </c>
-      <c r="G5" s="14">
+      <c r="H5" s="13">
         <v>1</v>
       </c>
-      <c r="H5" s="14">
+      <c r="I5" s="13">
         <v>-50</v>
       </c>
-      <c r="I5" s="14">
-        <f t="shared" ref="I5:I7" si="0">2*F5</f>
+      <c r="J5" s="13">
+        <f t="shared" ref="J5:J7" si="0">2*G5</f>
         <v>0.04</v>
       </c>
-      <c r="J5" s="15">
+      <c r="K5" s="14">
         <v>0.5</v>
       </c>
-      <c r="K5" s="15">
+      <c r="L5" s="14">
         <v>50</v>
       </c>
-      <c r="L5" s="15">
-        <v>0</v>
-      </c>
-      <c r="M5" s="16">
+      <c r="M5" s="14">
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
         <v>0.11</v>
       </c>
-      <c r="N5" s="16">
+      <c r="O5" s="15">
         <v>0.25</v>
       </c>
-      <c r="O5" s="16">
+      <c r="P5" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <f t="shared" ref="A6:A13" si="1">A5+1</f>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <f t="shared" ref="A6:A7" si="1">A5+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
         <v>5.0000000000000001E-9</v>
       </c>
-      <c r="D6" s="13">
+      <c r="E6" s="12">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E6" s="13">
+      <c r="F6" s="12">
         <v>-0.06</v>
       </c>
-      <c r="F6" s="13">
+      <c r="G6" s="12">
         <v>0.02</v>
       </c>
-      <c r="G6" s="14">
+      <c r="H6" s="13">
         <v>1</v>
       </c>
-      <c r="H6" s="14">
+      <c r="I6" s="13">
         <v>-50</v>
       </c>
-      <c r="I6" s="14">
+      <c r="J6" s="13">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="J6" s="15">
+      <c r="K6" s="14">
         <v>0.5</v>
       </c>
-      <c r="K6" s="15">
+      <c r="L6" s="14">
         <v>50</v>
       </c>
-      <c r="L6" s="15">
-        <v>0</v>
-      </c>
-      <c r="M6" s="16">
+      <c r="M6" s="14">
+        <v>0</v>
+      </c>
+      <c r="N6" s="15">
         <v>0.11</v>
       </c>
-      <c r="N6" s="16">
+      <c r="O6" s="15">
         <v>0.25</v>
       </c>
-      <c r="O6" s="16">
+      <c r="P6" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
         <v>5.0000000000000001E-9</v>
       </c>
-      <c r="D7" s="13">
+      <c r="E7" s="12">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E7" s="13">
+      <c r="F7" s="12">
         <v>-0.06</v>
       </c>
-      <c r="F7" s="13">
+      <c r="G7" s="12">
         <v>0.02</v>
       </c>
-      <c r="G7" s="14">
+      <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="H7" s="14">
+      <c r="I7" s="13">
         <v>-50</v>
       </c>
-      <c r="I7" s="14">
+      <c r="J7" s="13">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="J7" s="15">
+      <c r="K7" s="14">
         <v>0.5</v>
       </c>
-      <c r="K7" s="15">
+      <c r="L7" s="14">
         <v>50</v>
       </c>
-      <c r="L7" s="15">
-        <v>0</v>
-      </c>
-      <c r="M7" s="16">
+      <c r="M7" s="14">
+        <v>0</v>
+      </c>
+      <c r="N7" s="15">
         <v>0.11</v>
       </c>
-      <c r="N7" s="16">
+      <c r="O7" s="15">
         <v>0.25</v>
       </c>
-      <c r="O7" s="16">
+      <c r="P7" s="15">
         <v>0</v>
       </c>
     </row>

</xml_diff>